<commit_message>
ManhicaHDSS: Allow support for new Permanent ID (PermID) format ####-####, the number of houses increases to 9999
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/individual_details.xlsx
+++ b/xforms/xlsforms/individual_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8430" tabRatio="272" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8430" tabRatio="272"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -3611,7 +3611,7 @@
   <sheetPr/>
   <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="G50" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -6880,7 +6880,7 @@
   <sheetPr/>
   <dimension ref="A1:I291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>

</xml_diff>

<commit_message>
Individual Details Form: remove read-only flag in variables fatherName/motherName/spouseName
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/individual_details.xlsx
+++ b/xforms/xlsforms/individual_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8430" tabRatio="272"/>
+    <workbookView windowWidth="28695" windowHeight="13065" tabRatio="272"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1888,10 +1888,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -1922,25 +1922,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1958,19 +1952,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1989,17 +1983,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2013,16 +2005,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2036,6 +2042,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -2043,31 +2057,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2124,7 +2124,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2136,13 +2136,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2154,13 +2148,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2178,7 +2196,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2190,43 +2262,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2238,67 +2286,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2578,11 +2578,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2617,6 +2632,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2634,17 +2660,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -2656,22 +2671,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2680,146 +2680,146 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3267,10 +3267,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="141312"/>
+        <a:sysClr val="windowText" lastClr="232627"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="E0E9EE"/>
+        <a:sysClr val="window" lastClr="FCFCFC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3612,35 +3612,35 @@
   <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="$A20:$XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.9904761904762" customWidth="1"/>
-    <col min="2" max="2" width="27.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="50.9047619047619" style="86" customWidth="1"/>
-    <col min="4" max="4" width="42.4285714285714" style="86" customWidth="1"/>
-    <col min="5" max="5" width="26.4285714285714" style="86" customWidth="1"/>
-    <col min="6" max="6" width="41.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="43.8571428571429" style="86" customWidth="1"/>
-    <col min="8" max="8" width="45.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="42.1428571428571" customWidth="1"/>
-    <col min="10" max="10" width="30.8571428571429" customWidth="1"/>
-    <col min="11" max="11" width="96.3619047619048" customWidth="1"/>
-    <col min="12" max="12" width="50.4285714285714" customWidth="1"/>
-    <col min="13" max="13" width="44.1428571428571" customWidth="1"/>
-    <col min="14" max="14" width="12.4285714285714" customWidth="1"/>
-    <col min="15" max="15" width="15.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="29.9916666666667" customWidth="1"/>
+    <col min="2" max="2" width="27.1416666666667" customWidth="1"/>
+    <col min="3" max="3" width="50.9083333333333" style="86" customWidth="1"/>
+    <col min="4" max="4" width="42.425" style="86" customWidth="1"/>
+    <col min="5" max="5" width="26.425" style="86" customWidth="1"/>
+    <col min="6" max="6" width="41.2833333333333" customWidth="1"/>
+    <col min="7" max="7" width="43.8583333333333" style="86" customWidth="1"/>
+    <col min="8" max="8" width="45.8583333333333" customWidth="1"/>
+    <col min="9" max="9" width="42.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="30.8583333333333" customWidth="1"/>
+    <col min="11" max="11" width="96.3583333333333" customWidth="1"/>
+    <col min="12" max="12" width="50.425" customWidth="1"/>
+    <col min="13" max="13" width="44.1416666666667" customWidth="1"/>
+    <col min="14" max="14" width="12.425" customWidth="1"/>
+    <col min="15" max="15" width="15.7166666666667" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="13.7142857142857" customWidth="1"/>
-    <col min="18" max="18" width="13.8571428571429" customWidth="1"/>
-    <col min="19" max="19" width="20.1428571428571" customWidth="1"/>
-    <col min="20" max="20" width="21.1428571428571" customWidth="1"/>
+    <col min="17" max="17" width="13.7166666666667" customWidth="1"/>
+    <col min="18" max="18" width="13.8583333333333" customWidth="1"/>
+    <col min="19" max="19" width="20.1416666666667" customWidth="1"/>
+    <col min="20" max="20" width="21.1416666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:18">
@@ -4239,9 +4239,7 @@
       <c r="I20" s="90"/>
       <c r="J20" s="90"/>
       <c r="K20" s="90"/>
-      <c r="L20" s="92" t="b">
-        <v>1</v>
-      </c>
+      <c r="L20" s="92"/>
       <c r="M20" s="92"/>
       <c r="N20" s="90"/>
       <c r="O20" s="90"/>
@@ -4297,9 +4295,7 @@
       <c r="I22" s="90"/>
       <c r="J22" s="90"/>
       <c r="K22" s="90"/>
-      <c r="L22" s="92" t="b">
-        <v>1</v>
-      </c>
+      <c r="L22" s="92"/>
       <c r="M22" s="92"/>
       <c r="N22" s="90"/>
       <c r="O22" s="90"/>
@@ -4353,9 +4349,7 @@
       <c r="I24" s="90"/>
       <c r="J24" s="90"/>
       <c r="K24" s="90"/>
-      <c r="L24" s="92" t="b">
-        <v>1</v>
-      </c>
+      <c r="L24" s="92"/>
       <c r="M24" s="92"/>
       <c r="N24" s="90"/>
       <c r="O24" s="90"/>
@@ -6886,15 +6880,15 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7142857142857" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="13.7166666666667" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="29.1416666666667" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="24.2833333333333" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="6.57142857142857" customWidth="1"/>
-    <col min="7" max="7" width="26.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="37.7166666666667" customWidth="1"/>
+    <col min="6" max="6" width="6.575" customWidth="1"/>
+    <col min="7" max="7" width="26.1416666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1" spans="1:4">
@@ -10699,11 +10693,11 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42857142857143" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.425" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="24.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="23.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="32.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="24.7166666666667" customWidth="1"/>
+    <col min="2" max="2" width="23.2833333333333" customWidth="1"/>
+    <col min="3" max="3" width="32.2833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">

</xml_diff>